<commit_message>
Velocity parameter distribution loaded in R
</commit_message>
<xml_diff>
--- a/experimental_data/parameter_distributions/Koo_data.xlsx
+++ b/experimental_data/parameter_distributions/Koo_data.xlsx
@@ -8,7 +8,7 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="248" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Koo1975" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>Koo1975</t>
   </si>
@@ -58,13 +58,19 @@
     <t>cleaned data</t>
   </si>
   <si>
+    <t>[µm/s]</t>
+  </si>
+  <si>
+    <t>[-]</t>
+  </si>
+  <si>
     <t>range min</t>
   </si>
   <si>
     <t>range max</t>
   </si>
   <si>
-    <t>range midp</t>
+    <t>velocity</t>
   </si>
   <si>
     <t>SUM</t>
@@ -117,6 +123,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -127,6 +134,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -192,7 +200,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -210,6 +218,10 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -301,7 +313,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -315,7 +327,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Velocity Count</a:t>
             </a:r>
           </a:p>
@@ -333,7 +345,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Koo1975!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -352,36 +364,57 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$28:$M$34</c:f>
+              <c:f>Koo1975!$H$28:$H$41</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.05</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.65</c:v>
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1350</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$28:$D$35</c:f>
+              <c:f>Koo1975!$D$28:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -418,7 +451,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$4</c:f>
+              <c:f>Koo1975!$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -437,36 +470,57 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$28:$M$34</c:f>
+              <c:f>Koo1975!$H$28:$H$41</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.05</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.65</c:v>
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1350</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$28:$N$34</c:f>
+              <c:f>Koo1975!$N$28:$N$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -500,7 +554,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$4</c:f>
+              <c:f>Koo1975!$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -519,36 +573,57 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$28:$M$34</c:f>
+              <c:f>Koo1975!$H$28:$H$41</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.05</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.45</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.65</c:v>
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1350</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$28:$I$41</c:f>
+              <c:f>Koo1975!$I$28:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -599,11 +674,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="55422002"/>
-        <c:axId val="6900210"/>
+        <c:axId val="11691151"/>
+        <c:axId val="92210105"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55422002"/>
+        <c:axId val="11691151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,8 +694,8 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
-                  <a:t>RBC velocity (mm/s)</a:t>
+                  <a:rPr b="1" sz="900"/>
+                  <a:t>RBC velocity (µm/s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -637,14 +712,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="6900210"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="92210105"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6900210"/>
+        <c:axId val="92210105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +744,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>Count</a:t>
                 </a:r>
               </a:p>
@@ -687,8 +762,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55422002"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="11691151"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -725,15 +800,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>667080</xdr:colOff>
+      <xdr:colOff>694080</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>107280</xdr:colOff>
+      <xdr:colOff>133920</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -741,8 +816,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="667080" y="7620480"/>
-        <a:ext cx="7810560" cy="4937760"/>
+        <a:off x="694080" y="7579800"/>
+        <a:ext cx="7810200" cy="4746600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -762,8 +837,8 @@
   </sheetPr>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="N10" activeCellId="0" pane="topLeft" sqref="N10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="C27" activeCellId="0" pane="topLeft" sqref="C27:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -808,85 +883,85 @@
       <c r="L4" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.41</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="5" t="n">
         <v>0.35</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="5" t="n">
         <v>0.21</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.14</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="5" t="n">
         <v>0.21</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="5" t="n">
         <v>0.058</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="5" t="n">
         <v>139</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="5" t="n">
         <v>72</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="5" t="n">
         <v>304</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -897,10 +972,10 @@
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="K10" s="3" t="s">
@@ -911,713 +986,913 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="5" t="n">
         <v>0.042857144</v>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="8" t="n">
         <v>1.4210855E-014</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="5" t="n">
         <v>0.05154492</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="5" t="n">
         <v>11.114</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="5" t="n">
         <v>0.046925824</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="5" t="n">
         <v>20.577059</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="5" t="n">
         <v>0.14571428</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="5" t="n">
         <v>0.15644391</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="5" t="n">
         <v>20.019503</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="5" t="n">
         <v>0.15763585</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="5" t="n">
         <v>154.97542</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="5" t="n">
         <v>0.23714286</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="5" t="n">
         <v>0.24537</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="5" t="n">
         <v>3.9604633</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="5" t="n">
         <v>0.25708053</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="5" t="n">
         <v>101.95589</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="5" t="n">
         <v>0.34</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="5" t="n">
         <v>35.157894</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="5" t="n">
         <v>0.34746006</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="5" t="n">
         <v>12.97116</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="5" t="n">
         <v>0.34280047</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="5" t="n">
         <v>21.68615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="5" t="n">
         <v>0.44285715</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="5" t="n">
         <v>37.894737</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="5" t="n">
         <v>0.44551918</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="5" t="n">
         <v>5.932569</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="5" t="n">
         <v>0.44672748</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="5" t="n">
         <v>18.377462</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="5" t="n">
         <v>0.5485714</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="5" t="n">
         <v>24.631578</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="5" t="n">
         <v>0.54996586</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="5" t="n">
         <v>8.858814</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="5" t="n">
         <v>0.5494248</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16" s="5" t="n">
         <v>1.4312859</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="5" t="n">
         <v>0.6457143</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="5" t="n">
         <v>1.8947369</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="5" t="n">
         <v>0.64536685</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="5" t="n">
         <v>3.9185035</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="K17" s="5" t="n">
         <v>0.6534709</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17" s="5" t="n">
         <v>0.1764383</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="5" t="n">
         <v>0.7457143</v>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="8" t="n">
         <v>1.4210855E-014</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="5" t="n">
         <v>0.7438862</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="5" t="n">
         <v>2.9640684</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="5" t="n">
         <v>0.8426277</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="5" t="n">
         <v>4.9468117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="5" t="n">
         <v>0.9437973</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="5" t="n">
         <v>1.7891968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="5" t="n">
         <v>1.0422531</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="5" t="n">
         <v>-0.004432362</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="5" t="n">
         <v>1.1380271</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="5" t="n">
         <v>-0.0144790495</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="5" t="n">
         <v>1.2423865</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="5" t="n">
         <v>1.7578748</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="5" t="n">
         <v>1.3521178</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="5" t="n">
         <v>0.067962885</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
-      <c r="A26" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.9" outlineLevel="0" r="26">
+      <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="K26" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.9" outlineLevel="0" r="27">
+      <c r="C26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="H26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26" s="9"/>
+      <c r="M26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
       <c r="A27" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="6" t="s">
+      <c r="F27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="G27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>11</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N27" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
-      <c r="A28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B28" s="0" t="n">
+      <c r="A28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B28" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="C28" s="0" t="n">
-        <f aca="false">0.5*(A28+B28)</f>
-        <v>0.05</v>
-      </c>
-      <c r="D28" s="0" t="n">
+      <c r="C28" s="5" t="n">
+        <f aca="false">0.5*(A28+B28)*1000</f>
+        <v>50</v>
+      </c>
+      <c r="D28" s="5" t="n">
         <f aca="false">ROUND(B11)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" s="0" t="n">
+      <c r="F28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="H28" s="0" t="n">
-        <f aca="false">0.5*(F28+G28)</f>
-        <v>0.05</v>
-      </c>
-      <c r="I28" s="0" t="n">
+      <c r="H28" s="5" t="n">
+        <f aca="false">0.5*(F28+G28)*1000</f>
+        <v>50</v>
+      </c>
+      <c r="I28" s="5" t="n">
         <f aca="false">ROUND(G11)</f>
         <v>11</v>
       </c>
-      <c r="K28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" s="0" t="n">
+      <c r="K28" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="M28" s="0" t="n">
-        <f aca="false">0.5*(K28+L28)</f>
-        <v>0.05</v>
-      </c>
-      <c r="N28" s="0" t="n">
+      <c r="M28" s="5" t="n">
+        <f aca="false">0.5*(K28+L28)*1000</f>
+        <v>50</v>
+      </c>
+      <c r="N28" s="5" t="n">
         <f aca="false">ROUND(L11)</f>
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="C29" s="0" t="n">
-        <f aca="false">0.5*(A29+B29)</f>
-        <v>0.15</v>
-      </c>
-      <c r="D29" s="0" t="n">
+      <c r="C29" s="5" t="n">
+        <f aca="false">0.5*(A29+B29)*1000</f>
+        <v>150</v>
+      </c>
+      <c r="D29" s="5" t="n">
         <f aca="false">ROUND(B12)</f>
         <v>4</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="H29" s="0" t="n">
-        <f aca="false">0.5*(F29+G29)</f>
-        <v>0.15</v>
-      </c>
-      <c r="I29" s="0" t="n">
+      <c r="H29" s="5" t="n">
+        <f aca="false">0.5*(F29+G29)*1000</f>
+        <v>150</v>
+      </c>
+      <c r="I29" s="5" t="n">
         <f aca="false">ROUND(G12)</f>
         <v>20</v>
       </c>
-      <c r="K29" s="0" t="n">
+      <c r="K29" s="5" t="n">
         <v>0.1</v>
       </c>
-      <c r="L29" s="0" t="n">
+      <c r="L29" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="M29" s="0" t="n">
-        <f aca="false">0.5*(K29+L29)</f>
-        <v>0.15</v>
-      </c>
-      <c r="N29" s="0" t="n">
+      <c r="M29" s="5" t="n">
+        <f aca="false">0.5*(K29+L29)*1000</f>
+        <v>150</v>
+      </c>
+      <c r="N29" s="5" t="n">
         <f aca="false">ROUND(L12)</f>
         <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="C30" s="0" t="n">
-        <f aca="false">0.5*(A30+B30)</f>
-        <v>0.25</v>
-      </c>
-      <c r="D30" s="0" t="n">
+      <c r="C30" s="5" t="n">
+        <f aca="false">0.5*(A30+B30)*1000</f>
+        <v>250</v>
+      </c>
+      <c r="D30" s="5" t="n">
         <f aca="false">ROUND(B13)</f>
         <v>32</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="H30" s="0" t="n">
-        <f aca="false">0.5*(F30+G30)</f>
-        <v>0.25</v>
-      </c>
-      <c r="I30" s="0" t="n">
+      <c r="H30" s="5" t="n">
+        <f aca="false">0.5*(F30+G30)*1000</f>
+        <v>250</v>
+      </c>
+      <c r="I30" s="5" t="n">
         <f aca="false">ROUND(G13)</f>
         <v>4</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="K30" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="L30" s="0" t="n">
+      <c r="L30" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="M30" s="0" t="n">
-        <f aca="false">0.5*(K30+L30)</f>
-        <v>0.25</v>
-      </c>
-      <c r="N30" s="0" t="n">
+      <c r="M30" s="5" t="n">
+        <f aca="false">0.5*(K30+L30)*1000</f>
+        <v>250</v>
+      </c>
+      <c r="N30" s="5" t="n">
         <f aca="false">ROUND(L13)</f>
         <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="C31" s="0" t="n">
-        <f aca="false">0.5*(A31+B31)</f>
-        <v>0.35</v>
-      </c>
-      <c r="D31" s="0" t="n">
+      <c r="C31" s="5" t="n">
+        <f aca="false">0.5*(A31+B31)*1000</f>
+        <v>350</v>
+      </c>
+      <c r="D31" s="5" t="n">
         <f aca="false">ROUND(B14)</f>
         <v>35</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="H31" s="0" t="n">
-        <f aca="false">0.5*(F31+G31)</f>
-        <v>0.35</v>
-      </c>
-      <c r="I31" s="0" t="n">
+      <c r="H31" s="5" t="n">
+        <f aca="false">0.5*(F31+G31)*1000</f>
+        <v>350</v>
+      </c>
+      <c r="I31" s="5" t="n">
         <f aca="false">ROUND(G14)</f>
         <v>13</v>
       </c>
-      <c r="K31" s="0" t="n">
+      <c r="K31" s="5" t="n">
         <v>0.3</v>
       </c>
-      <c r="L31" s="0" t="n">
+      <c r="L31" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="M31" s="0" t="n">
-        <f aca="false">0.5*(K31+L31)</f>
-        <v>0.35</v>
-      </c>
-      <c r="N31" s="0" t="n">
+      <c r="M31" s="5" t="n">
+        <f aca="false">0.5*(K31+L31)*1000</f>
+        <v>350</v>
+      </c>
+      <c r="N31" s="5" t="n">
         <f aca="false">ROUND(L14)</f>
         <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="C32" s="0" t="n">
-        <f aca="false">0.5*(A32+B32)</f>
-        <v>0.45</v>
-      </c>
-      <c r="D32" s="0" t="n">
+      <c r="C32" s="5" t="n">
+        <f aca="false">0.5*(A32+B32)*1000</f>
+        <v>450</v>
+      </c>
+      <c r="D32" s="5" t="n">
         <f aca="false">ROUND(B15)</f>
         <v>38</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="H32" s="0" t="n">
-        <f aca="false">0.5*(F32+G32)</f>
-        <v>0.45</v>
-      </c>
-      <c r="I32" s="0" t="n">
+      <c r="H32" s="5" t="n">
+        <f aca="false">0.5*(F32+G32)*1000</f>
+        <v>450</v>
+      </c>
+      <c r="I32" s="5" t="n">
         <f aca="false">ROUND(G15)</f>
         <v>6</v>
       </c>
-      <c r="K32" s="0" t="n">
+      <c r="K32" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="L32" s="0" t="n">
+      <c r="L32" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="M32" s="0" t="n">
-        <f aca="false">0.5*(K32+L32)</f>
-        <v>0.45</v>
-      </c>
-      <c r="N32" s="0" t="n">
+      <c r="M32" s="5" t="n">
+        <f aca="false">0.5*(K32+L32)*1000</f>
+        <v>450</v>
+      </c>
+      <c r="N32" s="5" t="n">
         <f aca="false">ROUND(L15)</f>
         <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="5" t="n">
         <v>0.6</v>
       </c>
-      <c r="C33" s="0" t="n">
-        <f aca="false">0.5*(A33+B33)</f>
-        <v>0.55</v>
-      </c>
-      <c r="D33" s="0" t="n">
+      <c r="C33" s="5" t="n">
+        <f aca="false">0.5*(A33+B33)*1000</f>
+        <v>550</v>
+      </c>
+      <c r="D33" s="5" t="n">
         <f aca="false">ROUND(B16)</f>
         <v>25</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="G33" s="5" t="n">
         <v>0.6</v>
       </c>
-      <c r="H33" s="0" t="n">
-        <f aca="false">0.5*(F33+G33)</f>
-        <v>0.55</v>
-      </c>
-      <c r="I33" s="0" t="n">
+      <c r="H33" s="5" t="n">
+        <f aca="false">0.5*(F33+G33)*1000</f>
+        <v>550</v>
+      </c>
+      <c r="I33" s="5" t="n">
         <f aca="false">ROUND(G16)</f>
         <v>9</v>
       </c>
-      <c r="K33" s="0" t="n">
+      <c r="K33" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="L33" s="0" t="n">
+      <c r="L33" s="5" t="n">
         <v>0.6</v>
       </c>
-      <c r="M33" s="0" t="n">
-        <f aca="false">0.5*(K33+L33)</f>
-        <v>0.55</v>
-      </c>
-      <c r="N33" s="0" t="n">
+      <c r="M33" s="5" t="n">
+        <f aca="false">0.5*(K33+L33)*1000</f>
+        <v>550</v>
+      </c>
+      <c r="N33" s="5" t="n">
         <f aca="false">ROUND(L16)</f>
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="34">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="5" t="n">
         <v>0.6</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="5" t="n">
         <v>0.7</v>
       </c>
-      <c r="C34" s="0" t="n">
-        <f aca="false">0.5*(A34+B34)</f>
-        <v>0.65</v>
-      </c>
-      <c r="D34" s="0" t="n">
+      <c r="C34" s="5" t="n">
+        <f aca="false">0.5*(A34+B34)*1000</f>
+        <v>650</v>
+      </c>
+      <c r="D34" s="5" t="n">
         <f aca="false">ROUND(B17)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34" s="5" t="n">
         <v>0.6</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="5" t="n">
         <v>0.7</v>
       </c>
-      <c r="H34" s="0" t="n">
-        <f aca="false">0.5*(F34+G34)</f>
-        <v>0.65</v>
-      </c>
-      <c r="I34" s="0" t="n">
+      <c r="H34" s="5" t="n">
+        <f aca="false">0.5*(F34+G34)*1000</f>
+        <v>650</v>
+      </c>
+      <c r="I34" s="5" t="n">
         <f aca="false">ROUND(G17)</f>
         <v>4</v>
       </c>
-      <c r="K34" s="0" t="n">
+      <c r="K34" s="5" t="n">
         <v>0.6</v>
       </c>
-      <c r="L34" s="0" t="n">
+      <c r="L34" s="5" t="n">
         <v>0.7</v>
       </c>
-      <c r="M34" s="0" t="n">
-        <f aca="false">0.5*(K34+L34)</f>
-        <v>0.65</v>
-      </c>
-      <c r="N34" s="0" t="n">
+      <c r="M34" s="5" t="n">
+        <f aca="false">0.5*(K34+L34)*1000</f>
+        <v>650</v>
+      </c>
+      <c r="N34" s="5" t="n">
         <f aca="false">ROUND(L17)</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="35">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="5" t="n">
         <v>0.7</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="5" t="n">
         <v>0.8</v>
       </c>
-      <c r="C35" s="0" t="n">
-        <f aca="false">0.5*(A35+B35)</f>
-        <v>0.75</v>
-      </c>
-      <c r="D35" s="0" t="n">
+      <c r="C35" s="5" t="n">
+        <f aca="false">0.5*(A35+B35)*1000</f>
+        <v>750</v>
+      </c>
+      <c r="D35" s="5" t="n">
         <f aca="false">ROUND(B18)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35" s="5" t="n">
         <v>0.7</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35" s="5" t="n">
         <v>0.8</v>
       </c>
-      <c r="H35" s="0" t="n">
-        <f aca="false">0.5*(F35+G35)</f>
-        <v>0.75</v>
-      </c>
-      <c r="I35" s="0" t="n">
+      <c r="H35" s="5" t="n">
+        <f aca="false">0.5*(F35+G35)*1000</f>
+        <v>750</v>
+      </c>
+      <c r="I35" s="5" t="n">
         <f aca="false">ROUND(G18)</f>
         <v>3</v>
       </c>
-      <c r="M35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N35" s="8" t="n">
-        <f aca="false">SUM(N28:N34)</f>
-        <v>319</v>
+      <c r="K35" s="5" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L35" s="5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M35" s="5" t="n">
+        <f aca="false">0.5*(K35+L35)*1000</f>
+        <v>750</v>
+      </c>
+      <c r="N35" s="5" t="n">
+        <f aca="false">ROUND(L18)</f>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="36">
-      <c r="C36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="8" t="n">
-        <f aca="false">SUM(D28:D35)</f>
-        <v>136</v>
-      </c>
-      <c r="F36" s="0" t="n">
+      <c r="A36" s="5" t="n">
         <v>0.8</v>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="B36" s="5" t="n">
         <v>0.9</v>
       </c>
-      <c r="H36" s="0" t="n">
-        <f aca="false">0.5*(F36+G36)</f>
-        <v>0.85</v>
-      </c>
-      <c r="I36" s="0" t="n">
+      <c r="C36" s="5" t="n">
+        <f aca="false">0.5*(A36+B36)*1000</f>
+        <v>850</v>
+      </c>
+      <c r="D36" s="5" t="n">
+        <f aca="false">ROUND(B19)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G36" s="5" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="H36" s="5" t="n">
+        <f aca="false">0.5*(F36+G36)*1000</f>
+        <v>850</v>
+      </c>
+      <c r="I36" s="5" t="n">
         <f aca="false">ROUND(G19)</f>
         <v>5</v>
       </c>
+      <c r="K36" s="5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="L36" s="5" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M36" s="5" t="n">
+        <f aca="false">0.5*(K36+L36)*1000</f>
+        <v>850</v>
+      </c>
+      <c r="N36" s="5" t="n">
+        <f aca="false">ROUND(L19)</f>
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="37">
-      <c r="F37" s="0" t="n">
+      <c r="A37" s="5" t="n">
         <v>0.9</v>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="B37" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H37" s="0" t="n">
-        <f aca="false">0.5*(F37+G37)</f>
-        <v>0.95</v>
-      </c>
-      <c r="I37" s="0" t="n">
+      <c r="C37" s="5" t="n">
+        <f aca="false">0.5*(A37+B37)*1000</f>
+        <v>950</v>
+      </c>
+      <c r="D37" s="5" t="n">
+        <f aca="false">ROUND(B20)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="5" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G37" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5" t="n">
+        <f aca="false">0.5*(F37+G37)*1000</f>
+        <v>950</v>
+      </c>
+      <c r="I37" s="5" t="n">
         <f aca="false">ROUND(G20)</f>
         <v>2</v>
       </c>
+      <c r="K37" s="5" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L37" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M37" s="5" t="n">
+        <f aca="false">0.5*(K37+L37)*1000</f>
+        <v>950</v>
+      </c>
+      <c r="N37" s="5" t="n">
+        <f aca="false">ROUND(L20)</f>
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="38">
-      <c r="F38" s="0" t="n">
+      <c r="A38" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="B38" s="5" t="n">
         <v>1.1</v>
       </c>
-      <c r="H38" s="0" t="n">
-        <f aca="false">0.5*(F38+G38)</f>
-        <v>1.05</v>
-      </c>
-      <c r="I38" s="0" t="n">
+      <c r="C38" s="5" t="n">
+        <f aca="false">0.5*(A38+B38)*1000</f>
+        <v>1050</v>
+      </c>
+      <c r="D38" s="5" t="n">
+        <f aca="false">ROUND(B21)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="5" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H38" s="5" t="n">
+        <f aca="false">0.5*(F38+G38)*1000</f>
+        <v>1050</v>
+      </c>
+      <c r="I38" s="5" t="n">
         <f aca="false">ROUND(G21)</f>
         <v>-0</v>
       </c>
+      <c r="K38" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L38" s="5" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="M38" s="5" t="n">
+        <f aca="false">0.5*(K38+L38)*1000</f>
+        <v>1050</v>
+      </c>
+      <c r="N38" s="5" t="n">
+        <f aca="false">ROUND(L21)</f>
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
-      <c r="F39" s="0" t="n">
+      <c r="A39" s="5" t="n">
         <v>1.1</v>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="B39" s="5" t="n">
         <v>1.2</v>
       </c>
-      <c r="H39" s="0" t="n">
-        <f aca="false">0.5*(F39+G39)</f>
-        <v>1.15</v>
-      </c>
-      <c r="I39" s="0" t="n">
+      <c r="C39" s="5" t="n">
+        <f aca="false">0.5*(A39+B39)*1000</f>
+        <v>1150</v>
+      </c>
+      <c r="D39" s="5" t="n">
+        <f aca="false">ROUND(B22)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="5" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="G39" s="5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="H39" s="5" t="n">
+        <f aca="false">0.5*(F39+G39)*1000</f>
+        <v>1150</v>
+      </c>
+      <c r="I39" s="5" t="n">
         <f aca="false">ROUND(G22)</f>
         <v>-0</v>
       </c>
+      <c r="K39" s="5" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="L39" s="5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="M39" s="5" t="n">
+        <f aca="false">0.5*(K39+L39)*1000</f>
+        <v>1150</v>
+      </c>
+      <c r="N39" s="5" t="n">
+        <f aca="false">ROUND(L22)</f>
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="40">
-      <c r="F40" s="0" t="n">
+      <c r="A40" s="5" t="n">
         <v>1.2</v>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="B40" s="5" t="n">
         <v>1.3</v>
       </c>
-      <c r="H40" s="0" t="n">
-        <f aca="false">0.5*(F40+G40)</f>
-        <v>1.25</v>
-      </c>
-      <c r="I40" s="0" t="n">
+      <c r="C40" s="5" t="n">
+        <f aca="false">0.5*(A40+B40)*1000</f>
+        <v>1250</v>
+      </c>
+      <c r="D40" s="5" t="n">
+        <f aca="false">ROUND(B23)</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G40" s="5" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H40" s="5" t="n">
+        <f aca="false">0.5*(F40+G40)*1000</f>
+        <v>1250</v>
+      </c>
+      <c r="I40" s="5" t="n">
         <f aca="false">ROUND(G23)</f>
         <v>2</v>
       </c>
+      <c r="K40" s="5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="L40" s="5" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="M40" s="5" t="n">
+        <f aca="false">0.5*(K40+L40)*1000</f>
+        <v>1250</v>
+      </c>
+      <c r="N40" s="5" t="n">
+        <f aca="false">ROUND(L23)</f>
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="41">
-      <c r="F41" s="0" t="n">
+      <c r="A41" s="5" t="n">
         <v>1.3</v>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="B41" s="5" t="n">
         <v>1.4</v>
       </c>
-      <c r="H41" s="0" t="n">
-        <f aca="false">0.5*(F41+G41)</f>
-        <v>1.35</v>
-      </c>
-      <c r="I41" s="0" t="n">
+      <c r="C41" s="5" t="n">
+        <f aca="false">0.5*(A41+B41)*1000</f>
+        <v>1350</v>
+      </c>
+      <c r="D41" s="5" t="n">
+        <f aca="false">ROUND(B24)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="5" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G41" s="5" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H41" s="5" t="n">
+        <f aca="false">0.5*(F41+G41)*1000</f>
+        <v>1350</v>
+      </c>
+      <c r="I41" s="5" t="n">
         <f aca="false">ROUND(G24)</f>
         <v>0</v>
       </c>
+      <c r="K41" s="5" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="L41" s="5" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="M41" s="5" t="n">
+        <f aca="false">0.5*(K41+L41)*1000</f>
+        <v>1350</v>
+      </c>
+      <c r="N41" s="5" t="n">
+        <f aca="false">ROUND(L24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="42">
-      <c r="H42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="8" t="n">
+      <c r="C42" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="9" t="n">
+        <f aca="false">SUM(D28:D41)</f>
+        <v>136</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="9" t="n">
         <f aca="false">SUM(I28:I41)</f>
         <v>79</v>
+      </c>
+      <c r="M42" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N42" s="9" t="n">
+        <f aca="false">SUM(N28:N41)</f>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="48" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1631,17 +1906,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C27:D41 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.5748987854251"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
@@ -1660,12 +1942,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C27:D41 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="5" width="8.5748987854251"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>